<commit_message>
Update of GINF1 "Professeur"
</commit_message>
<xml_diff>
--- a/resources/GINF1/professeur.xlsx
+++ b/resources/GINF1/professeur.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\AP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D78FF2-BB99-4FB9-AD8A-68058CF13224}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53332FE-6761-4F69-923C-4A6DED818871}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5115" yWindow="2760" windowWidth="15375" windowHeight="8325" xr2:uid="{D282FDAF-2FDC-4854-80D2-C8EA3F1CCD5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>CIN</t>
   </si>
@@ -40,6 +40,48 @@
   </si>
   <si>
     <t>Matières enseignés</t>
+  </si>
+  <si>
+    <t>Tanana</t>
+  </si>
+  <si>
+    <t>Mariam</t>
+  </si>
+  <si>
+    <t>El Haddad</t>
+  </si>
+  <si>
+    <t>Mohamed</t>
+  </si>
+  <si>
+    <t>Khalid</t>
+  </si>
+  <si>
+    <t>Amechnoue</t>
+  </si>
+  <si>
+    <t>Massou</t>
+  </si>
+  <si>
+    <t>Siham</t>
+  </si>
+  <si>
+    <t>Belmokadem</t>
+  </si>
+  <si>
+    <t>Ghailani</t>
+  </si>
+  <si>
+    <t>Fissoune</t>
+  </si>
+  <si>
+    <t>Rachida</t>
+  </si>
+  <si>
+    <t>Nait Bouker</t>
+  </si>
+  <si>
+    <t>Nezha</t>
   </si>
 </sst>
 </file>
@@ -391,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8DE032-F837-48F3-9999-072D67E79C55}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,6 +463,67 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>